<commit_message>
changes according to acuity research module.
Signed-off-by: NitinNavatar <ngarg@navatargroup.com>
</commit_message>
<xml_diff>
--- a/ResearchDataSheet.xlsx
+++ b/ResearchDataSheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="276">
   <si>
     <t xml:space="preserve"> "     Advisorfirm NSAdmin Record04"</t>
   </si>
@@ -822,7 +822,37 @@
     <t>AR_Up3</t>
   </si>
   <si>
-    <t>Advisorcon05 Adm.rec05 - Updated</t>
+    <t>AR_Up4</t>
+  </si>
+  <si>
+    <t>Deal NSAdmin Company Record05</t>
+  </si>
+  <si>
+    <t>Deal NSAdmin Company Record05 - Updated</t>
+  </si>
+  <si>
+    <t>CompanyFund NSAdmin Record07</t>
+  </si>
+  <si>
+    <t>AR_Up5</t>
+  </si>
+  <si>
+    <t>Fundraising with Institution NSAdmin Record03</t>
+  </si>
+  <si>
+    <t>Fundraising with Institution NSAdmin Record03 - Updated</t>
+  </si>
+  <si>
+    <t>Intermediary  Type - TSK03</t>
+  </si>
+  <si>
+    <t>AR_Up6</t>
+  </si>
+  <si>
+    <t>AR_Up7</t>
+  </si>
+  <si>
+    <t>Intermediary  Type - Event03</t>
   </si>
 </sst>
 </file>
@@ -9193,17 +9223,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="41.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -9358,11 +9388,11 @@
       <c r="A3" t="s">
         <v>260</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s">
         <v>164</v>
       </c>
       <c r="D3">
-        <f>SUM(F3:U3)</f>
+        <f t="shared" ref="D3:D4" si="0">SUM(F3:U3)</f>
         <v>3</v>
       </c>
       <c r="E3" t="s">
@@ -9422,13 +9452,13 @@
         <v>264</v>
       </c>
       <c r="B4" t="s">
-        <v>164</v>
+        <v>266</v>
       </c>
       <c r="C4" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D4">
-        <f>SUM(F4:U4)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E4" t="s">
@@ -9481,6 +9511,261 @@
       </c>
       <c r="U4">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B5" t="s">
+        <v>268</v>
+      </c>
+      <c r="D5">
+        <f>SUM(F5:U5)</f>
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
+        <v>181</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>269</v>
+      </c>
+      <c r="B6" t="s">
+        <v>270</v>
+      </c>
+      <c r="C6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D6">
+        <f>SUM(F6:U6)</f>
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>181</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
+        <v>181</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>273</v>
+      </c>
+      <c r="B7" t="s">
+        <v>272</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:D8" si="1">SUM(F7:U7)</f>
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7" t="s">
+        <v>181</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>274</v>
+      </c>
+      <c r="B8" t="s">
+        <v>275</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>181</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
+        <v>181</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chnages according to module acuity research
Signed-off-by: NitinNavatar <ngarg@navatargroup.com>
</commit_message>
<xml_diff>
--- a/ResearchDataSheet.xlsx
+++ b/ResearchDataSheet.xlsx
@@ -14,6 +14,8 @@
   <sheets>
     <sheet name="SearchData" sheetId="1" r:id="rId1"/>
     <sheet name="UpdatedData" sheetId="2" r:id="rId2"/>
+    <sheet name="Others" sheetId="3" r:id="rId3"/>
+    <sheet name="UpdatedRecordType" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="353">
   <si>
     <t xml:space="preserve"> "     Advisorfirm NSAdmin Record04"</t>
   </si>
@@ -804,9 +806,6 @@
     <t>Variable_Name</t>
   </si>
   <si>
-    <t>Advisorfirm NSAdmin Record04</t>
-  </si>
-  <si>
     <t>AR_Up2</t>
   </si>
   <si>
@@ -825,41 +824,275 @@
     <t>AR_Up4</t>
   </si>
   <si>
-    <t>Deal NSAdmin Company Record05</t>
-  </si>
-  <si>
     <t>Deal NSAdmin Company Record05 - Updated</t>
   </si>
   <si>
-    <t>CompanyFund NSAdmin Record07</t>
-  </si>
-  <si>
     <t>AR_Up5</t>
   </si>
   <si>
-    <t>Fundraising with Institution NSAdmin Record03</t>
-  </si>
-  <si>
     <t>Fundraising with Institution NSAdmin Record03 - Updated</t>
   </si>
   <si>
-    <t>Intermediary  Type - TSK03</t>
-  </si>
-  <si>
     <t>AR_Up6</t>
   </si>
   <si>
     <t>AR_Up7</t>
   </si>
   <si>
-    <t>Intermediary  Type - Event03</t>
+    <t>Legal_Name</t>
+  </si>
+  <si>
+    <t>Record_Type</t>
+  </si>
+  <si>
+    <t>Other_LabelNames</t>
+  </si>
+  <si>
+    <t>Other_LabelValues</t>
+  </si>
+  <si>
+    <t>AR_Firm1</t>
+  </si>
+  <si>
+    <t>Consultant RT&lt;break&gt;IT Firm</t>
+  </si>
+  <si>
+    <t>AR_Deal1</t>
+  </si>
+  <si>
+    <t>AR_Contact1</t>
+  </si>
+  <si>
+    <t>Banker&lt;break&gt;Broker</t>
+  </si>
+  <si>
+    <t>Custom Contact Email&lt;break&gt;Custom Contact Phone&lt;break&gt;Custom Contact Text&lt;break&gt;Custom Contact TA&lt;break&gt;Custom Contact LTA&lt;break&gt;Custom Contact RTA</t>
+  </si>
+  <si>
+    <t>Email&lt;break&gt;Phone&lt;break&gt;Text&lt;break&gt;Text Area&lt;break&gt;Text Area (Long)&lt;break&gt;Text Area (Rich)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;break&gt; &lt;break&gt;255&lt;break&gt; &lt;break&gt;32768&lt;break&gt;32768</t>
+  </si>
+  <si>
+    <t>Field_Name</t>
+  </si>
+  <si>
+    <t>Data_Type</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>AR_Fund1</t>
+  </si>
+  <si>
+    <t>AR_Fundraising1</t>
+  </si>
+  <si>
+    <t>AR_Up8</t>
+  </si>
+  <si>
+    <t>Consultant RT</t>
+  </si>
+  <si>
+    <t>IT Firm</t>
+  </si>
+  <si>
+    <t>BuySide Deal</t>
+  </si>
+  <si>
+    <t>Capital Raise</t>
+  </si>
+  <si>
+    <t>SellSide Deal</t>
+  </si>
+  <si>
+    <t>Mutual Fund</t>
+  </si>
+  <si>
+    <t>Trust Fund</t>
+  </si>
+  <si>
+    <t>FRGRT</t>
+  </si>
+  <si>
+    <t>MSGRT</t>
+  </si>
+  <si>
+    <t>FRGRT&lt;break&gt;MSGRT</t>
+  </si>
+  <si>
+    <t>Mutual Fund&lt;break&gt;Trust Fund</t>
+  </si>
+  <si>
+    <t>BuySide Deal&lt;break&gt;SellSide Deal&lt;break&gt;Capital Raise</t>
+  </si>
+  <si>
+    <t>AR_NewFirm1</t>
+  </si>
+  <si>
+    <t>AR_NewFirm2</t>
+  </si>
+  <si>
+    <t>Tata Motor</t>
+  </si>
+  <si>
+    <t>GlobalLogic</t>
+  </si>
+  <si>
+    <t>AR_Up9</t>
+  </si>
+  <si>
+    <t>AR_Up10</t>
+  </si>
+  <si>
+    <t>AR_Up11</t>
+  </si>
+  <si>
+    <t>AR_Up12</t>
+  </si>
+  <si>
+    <t>AR_Up13</t>
+  </si>
+  <si>
+    <t>AR_Up14</t>
+  </si>
+  <si>
+    <t>AR_Up15</t>
+  </si>
+  <si>
+    <t>AR_Up16</t>
+  </si>
+  <si>
+    <t>AR_Up17</t>
+  </si>
+  <si>
+    <t>AR_Up18</t>
+  </si>
+  <si>
+    <t>"Advisorcon05 Adm.rec05"</t>
+  </si>
+  <si>
+    <t>"Actavis Generics"</t>
+  </si>
+  <si>
+    <t>"Clear Channel"</t>
+  </si>
+  <si>
+    <t>"Macquarie Group"</t>
+  </si>
+  <si>
+    <t>"Tata Motor"</t>
+  </si>
+  <si>
+    <t>"SellSide Deal"</t>
+  </si>
+  <si>
+    <t>"BuySide Deal"</t>
+  </si>
+  <si>
+    <t>"Capital Raise"</t>
+  </si>
+  <si>
+    <t>"Mutual Fund 2020"</t>
+  </si>
+  <si>
+    <t>"Trust Fund 2018"</t>
+  </si>
+  <si>
+    <t>AR_Up19</t>
+  </si>
+  <si>
+    <t>"Central Square Technologies" "Westpac Corporation"</t>
+  </si>
+  <si>
+    <t>Advisor&lt;break&gt;Company&lt;break&gt;Institution&lt;break&gt;Intermediary&lt;break&gt;Lender&lt;break&gt;Limited Partner&lt;break&gt;Portfolio Company</t>
+  </si>
+  <si>
+    <t>Advisor_Updated</t>
+  </si>
+  <si>
+    <t>Company_Updated</t>
+  </si>
+  <si>
+    <t>Institution_Updated</t>
+  </si>
+  <si>
+    <t>Intermediary_Updated</t>
+  </si>
+  <si>
+    <t>Lender_Updated</t>
+  </si>
+  <si>
+    <t>Limited Partner_Updated</t>
+  </si>
+  <si>
+    <t>Portfolio Company_Updated</t>
+  </si>
+  <si>
+    <t>Banker_Updated</t>
+  </si>
+  <si>
+    <t>Broker_Updated</t>
+  </si>
+  <si>
+    <t>BuySide Deal_Updated</t>
+  </si>
+  <si>
+    <t>Capital Raise_Updated</t>
+  </si>
+  <si>
+    <t>SellSide Deal_Updated</t>
+  </si>
+  <si>
+    <t>Mutual Fund_Updated</t>
+  </si>
+  <si>
+    <t>Trust Fund_Updated</t>
+  </si>
+  <si>
+    <t>FRGRT_Updated</t>
+  </si>
+  <si>
+    <t>MSGRT_Updated</t>
+  </si>
+  <si>
+    <t>ARURT_1</t>
+  </si>
+  <si>
+    <t>ARURT_2</t>
+  </si>
+  <si>
+    <t>ARURT_3</t>
+  </si>
+  <si>
+    <t>ARURT_4</t>
+  </si>
+  <si>
+    <t>AR_Up20</t>
+  </si>
+  <si>
+    <t>AR_Up21</t>
+  </si>
+  <si>
+    <t>AR_Up22</t>
+  </si>
+  <si>
+    <t>AR_Up23</t>
+  </si>
+  <si>
+    <t>AR_Up24</t>
+  </si>
+  <si>
+    <t>"Companycon01 Adm.rec01" "CompanyFund NSAdmin Record05"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -882,8 +1115,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -902,6 +1143,18 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -916,12 +1169,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1205,8 +1465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U131"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9223,42 +9483,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:AD25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="41.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="50.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="53.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="26" width="5.42578125" customWidth="1"/>
+    <col min="27" max="27" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>257</v>
@@ -9276,60 +9544,87 @@
         <v>253</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="V1" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="AA1" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B2" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
       <c r="C2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D2">
-        <f>SUM(F2:U2)</f>
+        <f>SUM(F2:AD2)</f>
         <v>6</v>
       </c>
       <c r="E2" t="s">
@@ -9341,8 +9636,8 @@
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2">
-        <v>0</v>
+      <c r="H2" t="s">
+        <v>181</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -9350,49 +9645,76 @@
       <c r="J2">
         <v>0</v>
       </c>
-      <c r="K2">
-        <v>0</v>
+      <c r="K2" t="s">
+        <v>181</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
         <v>2</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>1</v>
       </c>
-      <c r="O2" t="s">
-        <v>181</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
+      <c r="Q2" t="s">
+        <v>181</v>
+      </c>
+      <c r="R2" t="s">
+        <v>181</v>
+      </c>
+      <c r="S2" t="s">
+        <v>181</v>
+      </c>
+      <c r="T2" t="s">
+        <v>181</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W2" t="s">
+        <v>181</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
         <v>2</v>
       </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="AD2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>314</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D4" si="0">SUM(F3:U3)</f>
+        <f t="shared" ref="D3:D4" si="0">SUM(F3:AD3)</f>
         <v>3</v>
       </c>
       <c r="E3" t="s">
@@ -9404,8 +9726,8 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3">
-        <v>0</v>
+      <c r="H3" t="s">
+        <v>181</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -9413,8 +9735,8 @@
       <c r="J3">
         <v>0</v>
       </c>
-      <c r="K3">
-        <v>0</v>
+      <c r="K3" t="s">
+        <v>181</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -9423,39 +9745,66 @@
         <v>0</v>
       </c>
       <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
         <v>1</v>
       </c>
-      <c r="O3" t="s">
-        <v>181</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
+      <c r="Q3" t="s">
+        <v>181</v>
+      </c>
+      <c r="R3" t="s">
+        <v>181</v>
+      </c>
+      <c r="S3" t="s">
+        <v>181</v>
+      </c>
+      <c r="T3" t="s">
+        <v>181</v>
       </c>
       <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3" t="s">
+        <v>181</v>
+      </c>
+      <c r="W3" t="s">
+        <v>181</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B4" t="s">
-        <v>266</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
@@ -9470,8 +9819,8 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4">
-        <v>0</v>
+      <c r="H4" t="s">
+        <v>181</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -9479,8 +9828,8 @@
       <c r="J4">
         <v>0</v>
       </c>
-      <c r="K4">
-        <v>0</v>
+      <c r="K4" t="s">
+        <v>181</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -9489,228 +9838,336 @@
         <v>0</v>
       </c>
       <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
         <v>1</v>
       </c>
-      <c r="O4" t="s">
-        <v>181</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
+      <c r="Q4" t="s">
+        <v>181</v>
+      </c>
+      <c r="R4" t="s">
+        <v>181</v>
+      </c>
+      <c r="S4" t="s">
+        <v>181</v>
+      </c>
+      <c r="T4" t="s">
+        <v>181</v>
       </c>
       <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4" t="s">
+        <v>181</v>
+      </c>
+      <c r="W4" t="s">
+        <v>181</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5">
+        <f>SUM(F5:AD5)</f>
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>181</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>181</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>181</v>
+      </c>
+      <c r="R5" t="s">
+        <v>181</v>
+      </c>
+      <c r="S5" t="s">
+        <v>181</v>
+      </c>
+      <c r="T5" t="s">
+        <v>181</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5" t="s">
+        <v>181</v>
+      </c>
+      <c r="W5" t="s">
+        <v>181</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>266</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>267</v>
+      </c>
+      <c r="D6">
+        <f>SUM(F6:AD6)</f>
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>181</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>181</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>181</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>181</v>
+      </c>
+      <c r="R6" t="s">
+        <v>181</v>
+      </c>
+      <c r="S6" t="s">
+        <v>181</v>
+      </c>
+      <c r="T6" t="s">
+        <v>181</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6" t="s">
+        <v>181</v>
+      </c>
+      <c r="W6" t="s">
+        <v>181</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>268</v>
       </c>
-      <c r="D5">
-        <f>SUM(F5:U5)</f>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:D20" si="1">SUM(F7:AD7)</f>
         <v>1</v>
       </c>
-      <c r="E5" t="s">
-        <v>181</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5" t="s">
-        <v>181</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
+      <c r="E7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>181</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>181</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>181</v>
+      </c>
+      <c r="R7" t="s">
+        <v>181</v>
+      </c>
+      <c r="S7" t="s">
+        <v>181</v>
+      </c>
+      <c r="T7" t="s">
+        <v>181</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7" t="s">
+        <v>181</v>
+      </c>
+      <c r="W7" t="s">
+        <v>181</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
         <v>1</v>
       </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>269</v>
       </c>
-      <c r="B6" t="s">
-        <v>270</v>
-      </c>
-      <c r="C6" t="s">
-        <v>271</v>
-      </c>
-      <c r="D6">
-        <f>SUM(F6:U6)</f>
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>181</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6" t="s">
-        <v>181</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>273</v>
-      </c>
-      <c r="B7" t="s">
-        <v>272</v>
-      </c>
-      <c r="D7">
-        <f t="shared" ref="D7:D8" si="1">SUM(F7:U7)</f>
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>181</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7" t="s">
-        <v>181</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>1</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>274</v>
-      </c>
       <c r="B8" t="s">
-        <v>275</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
@@ -9725,8 +10182,8 @@
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8">
-        <v>0</v>
+      <c r="H8" t="s">
+        <v>181</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -9734,8 +10191,8 @@
       <c r="J8">
         <v>0</v>
       </c>
-      <c r="K8">
-        <v>0</v>
+      <c r="K8" t="s">
+        <v>181</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -9746,25 +10203,2213 @@
       <c r="N8">
         <v>0</v>
       </c>
-      <c r="O8" t="s">
-        <v>181</v>
+      <c r="O8">
+        <v>0</v>
       </c>
       <c r="P8">
         <v>0</v>
       </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
+      <c r="Q8" t="s">
+        <v>181</v>
+      </c>
+      <c r="R8" t="s">
+        <v>181</v>
+      </c>
+      <c r="S8" t="s">
+        <v>181</v>
+      </c>
+      <c r="T8" t="s">
+        <v>181</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8" t="s">
+        <v>181</v>
+      </c>
+      <c r="W8" t="s">
+        <v>181</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
         <v>1</v>
       </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>287</v>
+      </c>
+      <c r="B9" t="s">
+        <v>237</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>445</v>
+      </c>
+      <c r="E9" t="s">
+        <v>181</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <v>10</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>10</v>
+      </c>
+      <c r="M9">
+        <v>5</v>
+      </c>
+      <c r="N9">
+        <v>10</v>
+      </c>
+      <c r="O9">
+        <v>35</v>
+      </c>
+      <c r="P9">
+        <v>30</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>181</v>
+      </c>
+      <c r="R9">
+        <v>27</v>
+      </c>
+      <c r="S9">
+        <v>14</v>
+      </c>
+      <c r="T9">
+        <v>19</v>
+      </c>
+      <c r="U9" t="s">
+        <v>181</v>
+      </c>
+      <c r="V9">
+        <v>32</v>
+      </c>
+      <c r="W9">
+        <v>28</v>
+      </c>
+      <c r="X9" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y9">
+        <v>10</v>
+      </c>
+      <c r="Z9">
+        <v>10</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>175</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>304</v>
+      </c>
+      <c r="B10" t="s">
+        <v>318</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>181</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>181</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10" t="s">
+        <v>181</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>305</v>
+      </c>
+      <c r="B11" t="s">
+        <v>303</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>181</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>181</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11" t="s">
+        <v>181</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>306</v>
+      </c>
+      <c r="B12" t="s">
+        <v>315</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>181</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>181</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12" t="s">
+        <v>181</v>
+      </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y12">
+        <v>1</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>307</v>
+      </c>
+      <c r="B13" t="s">
+        <v>316</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>181</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>181</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="U13" t="s">
+        <v>181</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y13">
+        <v>1</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>308</v>
+      </c>
+      <c r="B14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>181</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>181</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14" t="s">
+        <v>181</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y14">
+        <v>1</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>309</v>
+      </c>
+      <c r="B15" t="s">
+        <v>319</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>181</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>181</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>9</v>
+      </c>
+      <c r="U15" t="s">
+        <v>181</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>310</v>
+      </c>
+      <c r="B16" t="s">
+        <v>320</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>181</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>181</v>
+      </c>
+      <c r="R16">
+        <v>9</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16" t="s">
+        <v>181</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>311</v>
+      </c>
+      <c r="B17" t="s">
+        <v>321</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>181</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>181</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>7</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17" t="s">
+        <v>181</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>312</v>
+      </c>
+      <c r="B18" t="s">
+        <v>322</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>181</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>181</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18" t="s">
+        <v>181</v>
+      </c>
+      <c r="V18">
+        <v>11</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>313</v>
+      </c>
+      <c r="B19" t="s">
+        <v>323</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>181</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>181</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19" t="s">
+        <v>181</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>14</v>
+      </c>
+      <c r="X19" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>324</v>
+      </c>
+      <c r="B20" t="s">
+        <v>325</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>181</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20" t="s">
+        <v>181</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y20">
+        <v>1</v>
+      </c>
+      <c r="Z20">
+        <v>1</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB20">
+        <v>0</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>347</v>
+      </c>
+      <c r="B21" t="s">
+        <v>229</v>
+      </c>
+      <c r="D21">
+        <f>SUM(E21:AD21)</f>
+        <v>140</v>
+      </c>
+      <c r="E21" t="s">
+        <v>181</v>
+      </c>
+      <c r="F21">
+        <v>15</v>
+      </c>
+      <c r="G21">
+        <v>15</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>15</v>
+      </c>
+      <c r="P21">
+        <v>15</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>181</v>
+      </c>
+      <c r="R21">
+        <v>9</v>
+      </c>
+      <c r="S21">
+        <v>4</v>
+      </c>
+      <c r="T21">
+        <v>17</v>
+      </c>
+      <c r="U21" t="s">
+        <v>181</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB21">
+        <v>0</v>
+      </c>
+      <c r="AC21">
+        <v>50</v>
+      </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>348</v>
+      </c>
+      <c r="B22" t="s">
+        <v>229</v>
+      </c>
+      <c r="D22">
+        <f>SUM(E22:AD22)</f>
+        <v>140</v>
+      </c>
+      <c r="E22" t="s">
+        <v>181</v>
+      </c>
+      <c r="F22">
+        <v>15</v>
+      </c>
+      <c r="G22">
+        <v>15</v>
+      </c>
+      <c r="H22" t="s">
+        <v>181</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
+        <v>181</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22" t="s">
+        <v>181</v>
+      </c>
+      <c r="P22" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q22">
+        <v>30</v>
+      </c>
+      <c r="R22" t="s">
+        <v>181</v>
+      </c>
+      <c r="S22" t="s">
+        <v>181</v>
+      </c>
+      <c r="T22" t="s">
+        <v>181</v>
+      </c>
+      <c r="U22">
+        <v>30</v>
+      </c>
+      <c r="V22" t="s">
+        <v>181</v>
+      </c>
+      <c r="W22" t="s">
+        <v>181</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA22">
+        <v>0</v>
+      </c>
+      <c r="AB22">
+        <v>0</v>
+      </c>
+      <c r="AC22">
+        <v>50</v>
+      </c>
+      <c r="AD22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>349</v>
+      </c>
+      <c r="B23" t="s">
+        <v>229</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ref="D23:D25" si="2">SUM(E23:U23)</f>
+        <v>90</v>
+      </c>
+      <c r="E23" t="s">
+        <v>181</v>
+      </c>
+      <c r="F23">
+        <v>15</v>
+      </c>
+      <c r="G23">
+        <v>15</v>
+      </c>
+      <c r="H23" t="s">
+        <v>181</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
+        <v>181</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>15</v>
+      </c>
+      <c r="P23">
+        <v>15</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>181</v>
+      </c>
+      <c r="R23" t="s">
+        <v>181</v>
+      </c>
+      <c r="S23" t="s">
+        <v>181</v>
+      </c>
+      <c r="T23" t="s">
+        <v>181</v>
+      </c>
+      <c r="U23">
+        <v>30</v>
+      </c>
+      <c r="V23" t="s">
+        <v>181</v>
+      </c>
+      <c r="W23" t="s">
+        <v>181</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <v>50</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>350</v>
+      </c>
+      <c r="B24" t="s">
+        <v>229</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="E24" t="s">
+        <v>181</v>
+      </c>
+      <c r="F24">
+        <v>15</v>
+      </c>
+      <c r="G24">
+        <v>15</v>
+      </c>
+      <c r="H24" t="s">
+        <v>181</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24" t="s">
+        <v>181</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24" t="s">
+        <v>181</v>
+      </c>
+      <c r="P24" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>181</v>
+      </c>
+      <c r="R24" t="s">
+        <v>181</v>
+      </c>
+      <c r="S24" t="s">
+        <v>181</v>
+      </c>
+      <c r="T24" t="s">
+        <v>181</v>
+      </c>
+      <c r="U24">
+        <v>30</v>
+      </c>
+      <c r="V24" t="s">
+        <v>181</v>
+      </c>
+      <c r="W24" t="s">
+        <v>181</v>
+      </c>
+      <c r="X24" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA24">
+        <v>0</v>
+      </c>
+      <c r="AB24">
+        <v>0</v>
+      </c>
+      <c r="AC24">
+        <v>50</v>
+      </c>
+      <c r="AD24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>351</v>
+      </c>
+      <c r="B25" t="s">
+        <v>352</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>181</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s">
+        <v>181</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25" t="s">
+        <v>181</v>
+      </c>
+      <c r="P25" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>181</v>
+      </c>
+      <c r="R25" t="s">
+        <v>181</v>
+      </c>
+      <c r="S25" t="s">
+        <v>181</v>
+      </c>
+      <c r="T25" t="s">
+        <v>181</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25" t="s">
+        <v>181</v>
+      </c>
+      <c r="W25" t="s">
+        <v>181</v>
+      </c>
+      <c r="X25" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA25">
+        <v>0</v>
+      </c>
+      <c r="AB25">
+        <v>0</v>
+      </c>
+      <c r="AC25">
+        <v>0</v>
+      </c>
+      <c r="AD25">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="149.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="119" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="149.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="90" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="E2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D2">
+        <f>SUM(E2:AD2)</f>
+        <v>140</v>
+      </c>
+      <c r="E2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F2">
+        <v>15</v>
+      </c>
+      <c r="G2">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>15</v>
+      </c>
+      <c r="P2">
+        <v>15</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>181</v>
+      </c>
+      <c r="R2">
+        <v>9</v>
+      </c>
+      <c r="S2">
+        <v>4</v>
+      </c>
+      <c r="T2">
+        <v>17</v>
+      </c>
+      <c r="U2" t="s">
+        <v>181</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>50</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>344</v>
+      </c>
+      <c r="B3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D5" si="0">SUM(F3:AD3)</f>
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>181</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3" t="s">
+        <v>181</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>345</v>
+      </c>
+      <c r="B4" t="s">
+        <v>316</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>181</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4" t="s">
+        <v>181</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>346</v>
+      </c>
+      <c r="B5" t="s">
+        <v>317</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>181</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5" t="s">
+        <v>181</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes according to Module Acuity Research.
Signed-off-by: NitinNavatar <ngarg@navatargroup.com>
</commit_message>
<xml_diff>
--- a/ResearchDataSheet.xlsx
+++ b/ResearchDataSheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="357">
   <si>
     <t xml:space="preserve"> "     Advisorfirm NSAdmin Record04"</t>
   </si>
@@ -1086,6 +1086,18 @@
   </si>
   <si>
     <t>"Companycon01 Adm.rec01" "CompanyFund NSAdmin Record05"</t>
+  </si>
+  <si>
+    <t>AR_Up25</t>
+  </si>
+  <si>
+    <t>AR_Up26</t>
+  </si>
+  <si>
+    <t>AR_Up27</t>
+  </si>
+  <si>
+    <t>AR_Up28</t>
   </si>
 </sst>
 </file>
@@ -9483,10 +9495,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD25"/>
+  <dimension ref="A1:AD29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11430,7 +11442,7 @@
         <v>229</v>
       </c>
       <c r="D22">
-        <f>SUM(E22:AD22)</f>
+        <f t="shared" ref="D22:D29" si="2">SUM(E22:AD22)</f>
         <v>140</v>
       </c>
       <c r="E22" t="s">
@@ -11520,8 +11532,8 @@
         <v>229</v>
       </c>
       <c r="D23">
-        <f t="shared" ref="D23:D25" si="2">SUM(E23:U23)</f>
-        <v>90</v>
+        <f t="shared" si="2"/>
+        <v>140</v>
       </c>
       <c r="E23" t="s">
         <v>181</v>
@@ -11611,7 +11623,7 @@
       </c>
       <c r="D24">
         <f t="shared" si="2"/>
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="E24" t="s">
         <v>181</v>
@@ -11779,6 +11791,366 @@
         <v>0</v>
       </c>
       <c r="AD25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>353</v>
+      </c>
+      <c r="B26">
+        <v>56789012</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>95</v>
+      </c>
+      <c r="E26" t="s">
+        <v>181</v>
+      </c>
+      <c r="F26">
+        <v>15</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26" t="s">
+        <v>181</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26" t="s">
+        <v>181</v>
+      </c>
+      <c r="L26">
+        <v>15</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>15</v>
+      </c>
+      <c r="P26">
+        <v>15</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>181</v>
+      </c>
+      <c r="R26" t="s">
+        <v>181</v>
+      </c>
+      <c r="S26" t="s">
+        <v>181</v>
+      </c>
+      <c r="T26" t="s">
+        <v>181</v>
+      </c>
+      <c r="U26">
+        <v>15</v>
+      </c>
+      <c r="V26" t="s">
+        <v>181</v>
+      </c>
+      <c r="W26" t="s">
+        <v>181</v>
+      </c>
+      <c r="X26">
+        <v>15</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA26">
+        <v>0</v>
+      </c>
+      <c r="AB26">
+        <v>0</v>
+      </c>
+      <c r="AC26">
+        <v>0</v>
+      </c>
+      <c r="AD26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>354</v>
+      </c>
+      <c r="B27">
+        <v>56789012</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="E27" t="s">
+        <v>181</v>
+      </c>
+      <c r="F27">
+        <v>15</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27" t="s">
+        <v>181</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27" t="s">
+        <v>181</v>
+      </c>
+      <c r="L27">
+        <v>15</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>181</v>
+      </c>
+      <c r="R27" t="s">
+        <v>181</v>
+      </c>
+      <c r="S27" t="s">
+        <v>181</v>
+      </c>
+      <c r="T27" t="s">
+        <v>181</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27" t="s">
+        <v>181</v>
+      </c>
+      <c r="W27" t="s">
+        <v>181</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+      <c r="AC27">
+        <v>0</v>
+      </c>
+      <c r="AD27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>355</v>
+      </c>
+      <c r="B28" t="s">
+        <v>235</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>445</v>
+      </c>
+      <c r="E28" t="s">
+        <v>181</v>
+      </c>
+      <c r="F28">
+        <v>10</v>
+      </c>
+      <c r="G28">
+        <v>10</v>
+      </c>
+      <c r="H28" t="s">
+        <v>181</v>
+      </c>
+      <c r="I28">
+        <v>10</v>
+      </c>
+      <c r="J28">
+        <v>10</v>
+      </c>
+      <c r="K28" t="s">
+        <v>181</v>
+      </c>
+      <c r="L28">
+        <v>10</v>
+      </c>
+      <c r="M28">
+        <v>5</v>
+      </c>
+      <c r="N28">
+        <v>10</v>
+      </c>
+      <c r="O28">
+        <v>35</v>
+      </c>
+      <c r="P28">
+        <v>30</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>181</v>
+      </c>
+      <c r="R28" t="s">
+        <v>181</v>
+      </c>
+      <c r="S28" t="s">
+        <v>181</v>
+      </c>
+      <c r="T28" t="s">
+        <v>181</v>
+      </c>
+      <c r="U28">
+        <v>60</v>
+      </c>
+      <c r="V28" t="s">
+        <v>181</v>
+      </c>
+      <c r="W28" t="s">
+        <v>181</v>
+      </c>
+      <c r="X28">
+        <v>60</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA28">
+        <v>20</v>
+      </c>
+      <c r="AB28">
+        <v>0</v>
+      </c>
+      <c r="AC28">
+        <v>175</v>
+      </c>
+      <c r="AD28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>356</v>
+      </c>
+      <c r="B29" t="s">
+        <v>199</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="E29" t="s">
+        <v>181</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>15</v>
+      </c>
+      <c r="H29" t="s">
+        <v>181</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29" t="s">
+        <v>181</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>181</v>
+      </c>
+      <c r="R29" t="s">
+        <v>181</v>
+      </c>
+      <c r="S29" t="s">
+        <v>181</v>
+      </c>
+      <c r="T29" t="s">
+        <v>181</v>
+      </c>
+      <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29" t="s">
+        <v>181</v>
+      </c>
+      <c r="W29" t="s">
+        <v>181</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA29">
+        <v>0</v>
+      </c>
+      <c r="AB29">
+        <v>20</v>
+      </c>
+      <c r="AC29">
+        <v>0</v>
+      </c>
+      <c r="AD29">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes according to phase 2 org for Module Acuity Research
Signed-off-by: NitinNavatar <ngarg@navatargroup.com>
</commit_message>
<xml_diff>
--- a/ResearchDataSheet.xlsx
+++ b/ResearchDataSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SearchData" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,9 @@
     <sheet name="Others" sheetId="3" r:id="rId3"/>
     <sheet name="UpdatedRecordType" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SearchData!$C$1:$X$131</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="413">
   <si>
     <t>ACR_130</t>
   </si>
@@ -640,9 +643,6 @@
     <t>ACR_22</t>
   </si>
   <si>
-    <t>"56789012 2123123"</t>
-  </si>
-  <si>
     <t>ACR_21</t>
   </si>
   <si>
@@ -730,9 +730,6 @@
     <t>ACR_5</t>
   </si>
   <si>
-    <t>"Advisorfirm NSAdmin Record04"</t>
-  </si>
-  <si>
     <t>ACR_4</t>
   </si>
   <si>
@@ -754,12 +751,6 @@
     <t>ACR_1</t>
   </si>
   <si>
-    <t>Referenced Contacts</t>
-  </si>
-  <si>
-    <t>Referenced Accounts</t>
-  </si>
-  <si>
     <t>Interactions</t>
   </si>
   <si>
@@ -979,9 +970,6 @@
     <t>AR_Up18</t>
   </si>
   <si>
-    <t>"Advisorcon05 Adm.rec05"</t>
-  </si>
-  <si>
     <t>"Actavis Generics"</t>
   </si>
   <si>
@@ -1253,6 +1241,45 @@
   </si>
   <si>
     <t>Files</t>
+  </si>
+  <si>
+    <t>Advisorfirm NSAdmin Record04</t>
+  </si>
+  <si>
+    <t>Tagged Accounts</t>
+  </si>
+  <si>
+    <t>Tagged Contacts</t>
+  </si>
+  <si>
+    <t>56789012 2123123</t>
+  </si>
+  <si>
+    <t>Intermediary  Type - TSK03</t>
+  </si>
+  <si>
+    <t>Intermediary  Type - Event03</t>
+  </si>
+  <si>
+    <t>Intermediary  Type - Event03 Updated</t>
+  </si>
+  <si>
+    <t>Intermediary  Type - TSK03 Updated</t>
+  </si>
+  <si>
+    <t>CompanyFund NSAdmin Record07 - Updated</t>
+  </si>
+  <si>
+    <t>CompanyFund NSAdmin Record07</t>
+  </si>
+  <si>
+    <t>Fundraising with Institution NSAdmin Record03</t>
+  </si>
+  <si>
+    <t>Deal NSAdmin Company Record05</t>
+  </si>
+  <si>
+    <t>Advisorcon05 Adm.rec05 - Updated</t>
   </si>
 </sst>
 </file>
@@ -1632,8 +1659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X131"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3:U131"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1663,82 +1690,82 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="S1" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>402</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D33" si="0">SUM(E2:X2)</f>
@@ -1807,10 +1834,10 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
@@ -1879,10 +1906,10 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
@@ -1951,10 +1978,10 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C5" t="s">
-        <v>230</v>
+        <v>400</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
@@ -2023,10 +2050,10 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
@@ -2095,10 +2122,10 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -2167,10 +2194,10 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -2239,7 +2266,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C9">
         <v>3434343434</v>
@@ -2311,10 +2338,10 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C10">
-        <v>4545</v>
+        <v>45454</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
@@ -2383,10 +2410,10 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
@@ -2455,10 +2482,10 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -2527,10 +2554,10 @@
     </row>
     <row r="13" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
@@ -2599,10 +2626,10 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
@@ -2671,10 +2698,10 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
@@ -2743,10 +2770,10 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
@@ -2815,10 +2842,10 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
@@ -2887,10 +2914,10 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
@@ -2959,10 +2986,10 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
@@ -3031,7 +3058,7 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C20">
         <v>56789012</v>
@@ -3103,7 +3130,7 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C21">
         <v>56789</v>
@@ -3175,10 +3202,10 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C22" t="s">
-        <v>200</v>
+        <v>403</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
@@ -4049,35 +4076,35 @@
         <f t="shared" ref="D34:D65" si="1">SUM(E34:X34)</f>
         <v>0</v>
       </c>
-      <c r="E34" t="s">
-        <v>180</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
-      <c r="K34">
-        <v>0</v>
-      </c>
-      <c r="L34">
-        <v>0</v>
-      </c>
-      <c r="M34">
-        <v>0</v>
-      </c>
-      <c r="N34">
-        <v>0</v>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>180</v>
+      </c>
+      <c r="G34" t="s">
+        <v>180</v>
+      </c>
+      <c r="H34" t="s">
+        <v>180</v>
+      </c>
+      <c r="I34" t="s">
+        <v>180</v>
+      </c>
+      <c r="J34" t="s">
+        <v>180</v>
+      </c>
+      <c r="K34" t="s">
+        <v>180</v>
+      </c>
+      <c r="L34" t="s">
+        <v>180</v>
+      </c>
+      <c r="M34" t="s">
+        <v>180</v>
+      </c>
+      <c r="N34" t="s">
+        <v>180</v>
       </c>
       <c r="O34">
         <v>0</v>
@@ -4122,35 +4149,35 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E35" t="s">
-        <v>180</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
-      <c r="K35">
-        <v>0</v>
-      </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
-      <c r="M35">
-        <v>0</v>
-      </c>
-      <c r="N35">
-        <v>0</v>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>180</v>
+      </c>
+      <c r="G35" t="s">
+        <v>180</v>
+      </c>
+      <c r="H35" t="s">
+        <v>180</v>
+      </c>
+      <c r="I35" t="s">
+        <v>180</v>
+      </c>
+      <c r="J35" t="s">
+        <v>180</v>
+      </c>
+      <c r="K35" t="s">
+        <v>180</v>
+      </c>
+      <c r="L35" t="s">
+        <v>180</v>
+      </c>
+      <c r="M35" t="s">
+        <v>180</v>
+      </c>
+      <c r="N35" t="s">
+        <v>180</v>
       </c>
       <c r="O35">
         <v>0</v>
@@ -4195,35 +4222,35 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E36" t="s">
-        <v>180</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
-      <c r="K36">
-        <v>0</v>
-      </c>
-      <c r="L36">
-        <v>0</v>
-      </c>
-      <c r="M36">
-        <v>0</v>
-      </c>
-      <c r="N36">
-        <v>0</v>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>180</v>
+      </c>
+      <c r="G36" t="s">
+        <v>180</v>
+      </c>
+      <c r="H36" t="s">
+        <v>180</v>
+      </c>
+      <c r="I36" t="s">
+        <v>180</v>
+      </c>
+      <c r="J36" t="s">
+        <v>180</v>
+      </c>
+      <c r="K36" t="s">
+        <v>180</v>
+      </c>
+      <c r="L36" t="s">
+        <v>180</v>
+      </c>
+      <c r="M36" t="s">
+        <v>180</v>
+      </c>
+      <c r="N36" t="s">
+        <v>180</v>
       </c>
       <c r="O36">
         <v>0</v>
@@ -4268,35 +4295,35 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E37" t="s">
-        <v>180</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
-      <c r="K37">
-        <v>0</v>
-      </c>
-      <c r="L37">
-        <v>0</v>
-      </c>
-      <c r="M37">
-        <v>0</v>
-      </c>
-      <c r="N37">
-        <v>0</v>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>180</v>
+      </c>
+      <c r="G37" t="s">
+        <v>180</v>
+      </c>
+      <c r="H37" t="s">
+        <v>180</v>
+      </c>
+      <c r="I37" t="s">
+        <v>180</v>
+      </c>
+      <c r="J37" t="s">
+        <v>180</v>
+      </c>
+      <c r="K37" t="s">
+        <v>180</v>
+      </c>
+      <c r="L37" t="s">
+        <v>180</v>
+      </c>
+      <c r="M37" t="s">
+        <v>180</v>
+      </c>
+      <c r="N37" t="s">
+        <v>180</v>
       </c>
       <c r="O37">
         <v>0</v>
@@ -8208,34 +8235,37 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E94" t="s">
-        <v>180</v>
-      </c>
-      <c r="F94">
-        <v>0</v>
-      </c>
-      <c r="G94">
-        <v>0</v>
-      </c>
-      <c r="H94">
-        <v>0</v>
-      </c>
-      <c r="I94">
-        <v>0</v>
-      </c>
-      <c r="J94">
-        <v>0</v>
-      </c>
-      <c r="K94">
-        <v>0</v>
-      </c>
-      <c r="L94">
-        <v>0</v>
-      </c>
-      <c r="M94">
-        <v>0</v>
-      </c>
-      <c r="N94">
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94" t="s">
+        <v>180</v>
+      </c>
+      <c r="G94" t="s">
+        <v>180</v>
+      </c>
+      <c r="H94" t="s">
+        <v>180</v>
+      </c>
+      <c r="I94" t="s">
+        <v>180</v>
+      </c>
+      <c r="J94" t="s">
+        <v>180</v>
+      </c>
+      <c r="K94" t="s">
+        <v>180</v>
+      </c>
+      <c r="L94" t="s">
+        <v>180</v>
+      </c>
+      <c r="M94" t="s">
+        <v>180</v>
+      </c>
+      <c r="N94" t="s">
+        <v>180</v>
+      </c>
+      <c r="O94">
         <v>0</v>
       </c>
       <c r="P94">
@@ -10755,7 +10785,7 @@
         <v>0</v>
       </c>
       <c r="C131" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="D131">
         <f t="shared" si="4"/>
@@ -10820,6 +10850,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="C1:X131"/>
   <hyperlinks>
     <hyperlink ref="C55" r:id="rId1"/>
   </hyperlinks>
@@ -10832,8 +10863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG54"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AB3" sqref="AB3:AD54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10871,114 +10902,114 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="U1" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="R1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="X1" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="U1" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>295</v>
-      </c>
       <c r="AA1" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="AB1" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="AG1" s="2" t="s">
         <v>402</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B2" t="s">
-        <v>230</v>
+        <v>400</v>
       </c>
       <c r="C2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D20" si="0">SUM(F2:AG2)</f>
@@ -11074,10 +11105,13 @@
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B3" t="s">
-        <v>313</v>
+        <v>163</v>
+      </c>
+      <c r="C3" t="s">
+        <v>412</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
@@ -11173,13 +11207,13 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>411</v>
       </c>
       <c r="C4" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
@@ -11275,10 +11309,13 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>409</v>
+      </c>
+      <c r="C5" t="s">
+        <v>408</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
@@ -11374,13 +11411,13 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>410</v>
       </c>
       <c r="C6" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
@@ -11476,10 +11513,13 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>404</v>
+      </c>
+      <c r="C7" t="s">
+        <v>407</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -11575,10 +11615,13 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>405</v>
+      </c>
+      <c r="C8" t="s">
+        <v>406</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -11674,10 +11717,10 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B9" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
@@ -11773,10 +11816,10 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B10" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
@@ -11872,10 +11915,10 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B11" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
@@ -11971,10 +12014,10 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B12" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -12070,10 +12113,10 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B13" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
@@ -12169,10 +12212,10 @@
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B14" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
@@ -12268,10 +12311,10 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B15" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
@@ -12367,10 +12410,10 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B16" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
@@ -12466,10 +12509,10 @@
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B17" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
@@ -12565,10 +12608,10 @@
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B18" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
@@ -12664,10 +12707,10 @@
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B19" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
@@ -12763,10 +12806,10 @@
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B20" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
@@ -12862,10 +12905,10 @@
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="B21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D21">
         <f>SUM(E21:AG21)</f>
@@ -12961,10 +13004,10 @@
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D22">
         <f t="shared" ref="D22:D52" si="1">SUM(E22:AG22)</f>
@@ -13060,10 +13103,10 @@
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
@@ -13159,10 +13202,10 @@
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
@@ -13258,10 +13301,10 @@
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B25" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
@@ -13357,7 +13400,7 @@
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B26">
         <v>56789012</v>
@@ -13456,7 +13499,7 @@
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B27">
         <v>56789012</v>
@@ -13555,10 +13598,10 @@
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B28" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D28">
         <f t="shared" si="1"/>
@@ -13654,7 +13697,7 @@
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B29" t="s">
         <v>198</v>
@@ -13753,10 +13796,10 @@
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="B30" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D30">
         <f t="shared" si="1"/>
@@ -13852,10 +13895,10 @@
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D31">
         <f t="shared" si="1"/>
@@ -13951,7 +13994,7 @@
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B32" t="s">
         <v>17</v>
@@ -14050,10 +14093,10 @@
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B33" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="D33">
         <f t="shared" si="1"/>
@@ -14149,10 +14192,10 @@
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="B34" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D34">
         <f t="shared" si="1"/>
@@ -14248,10 +14291,10 @@
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B35" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D35">
         <f t="shared" si="1"/>
@@ -14347,10 +14390,10 @@
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B36" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="D36">
         <f t="shared" si="1"/>
@@ -14446,10 +14489,10 @@
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B37" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D37">
         <f t="shared" si="1"/>
@@ -14545,10 +14588,10 @@
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="B38" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="D38">
         <f t="shared" si="1"/>
@@ -14644,10 +14687,10 @@
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="B39" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="D39">
         <f t="shared" si="1"/>
@@ -14743,10 +14786,10 @@
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>353</v>
+      </c>
+      <c r="B40" t="s">
         <v>358</v>
-      </c>
-      <c r="B40" t="s">
-        <v>363</v>
       </c>
       <c r="D40">
         <f t="shared" si="1"/>
@@ -14842,10 +14885,10 @@
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>354</v>
+      </c>
+      <c r="B41" t="s">
         <v>359</v>
-      </c>
-      <c r="B41" t="s">
-        <v>364</v>
       </c>
       <c r="D41">
         <f t="shared" si="1"/>
@@ -14941,10 +14984,10 @@
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>355</v>
+      </c>
+      <c r="B42" t="s">
         <v>360</v>
-      </c>
-      <c r="B42" t="s">
-        <v>365</v>
       </c>
       <c r="D42">
         <f t="shared" si="1"/>
@@ -15040,10 +15083,10 @@
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>356</v>
+      </c>
+      <c r="B43" t="s">
         <v>361</v>
-      </c>
-      <c r="B43" t="s">
-        <v>366</v>
       </c>
       <c r="D43">
         <f t="shared" si="1"/>
@@ -15139,10 +15182,10 @@
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>357</v>
+      </c>
+      <c r="B44" t="s">
         <v>362</v>
-      </c>
-      <c r="B44" t="s">
-        <v>367</v>
       </c>
       <c r="D44">
         <f t="shared" si="1"/>
@@ -15238,10 +15281,10 @@
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="B45" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D45">
         <f t="shared" si="1"/>
@@ -15337,10 +15380,10 @@
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="B46" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D46">
         <f t="shared" si="1"/>
@@ -15436,10 +15479,10 @@
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="B47" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D47">
         <f t="shared" si="1"/>
@@ -15535,10 +15578,10 @@
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="B48" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="D48">
         <f t="shared" si="1"/>
@@ -15634,10 +15677,10 @@
     </row>
     <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="B49" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="D49">
         <f t="shared" si="1"/>
@@ -15733,7 +15776,7 @@
     </row>
     <row r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B50" t="s">
         <v>165</v>
@@ -15832,10 +15875,10 @@
     </row>
     <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="B51" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="D51">
         <f t="shared" si="1"/>
@@ -15931,10 +15974,10 @@
     </row>
     <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="B52" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="D52">
         <f t="shared" si="1"/>
@@ -16030,10 +16073,10 @@
     </row>
     <row r="53" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="B53" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -16128,10 +16171,10 @@
     </row>
     <row r="54" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="B54" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -16255,109 +16298,109 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -16369,8 +16412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AB3" sqref="AB3:AD5"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AF1" sqref="AF1:AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16410,111 +16453,111 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="U1" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="R1" s="2" t="s">
+      <c r="X1" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="T1" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="V1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB1" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="X1" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="Z1" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="AG1" s="2" t="s">
         <v>402</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D2">
         <f>SUM(E2:AG2)</f>
@@ -16610,10 +16653,10 @@
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B3" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D5" si="0">SUM(F3:AG3)</f>
@@ -16709,10 +16752,10 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B4" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
@@ -16808,10 +16851,10 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B5" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Updated research Data sheet
Signed-off-by: Nitin Garg <ngarg@navatargroup.com>
</commit_message>
<xml_diff>
--- a/ResearchDataSheet.xlsx
+++ b/ResearchDataSheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravi Kumar\git\PE4.7Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nitin Garg\git\PE4.7Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B2F061-B19C-4754-8F92-FFC5BCBB57AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchData" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SearchData!$C$1:$Y$132</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1360,7 +1361,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1465,7 +1466,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1480,10 +1481,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1760,39 +1762,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y132"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="55.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="42.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="15" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="22" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="55.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="42.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="15" width="18.44140625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="5.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="22" width="11.33203125" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1867,7 +1869,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1876,7 +1878,7 @@
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D33" si="0">SUM(E2:Y2)</f>
-        <v>452</v>
+        <v>828</v>
       </c>
       <c r="E2" t="s">
         <v>26</v>
@@ -1906,7 +1908,7 @@
         <v>10</v>
       </c>
       <c r="N2">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="O2">
         <v>30</v>
@@ -1915,10 +1917,10 @@
         <v>26</v>
       </c>
       <c r="Q2">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="R2">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="S2">
         <v>20</v>
@@ -1930,19 +1932,19 @@
         <v>10</v>
       </c>
       <c r="V2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="X2" s="7">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="Y2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1951,7 +1953,7 @@
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>452</v>
+        <v>828</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -1981,7 +1983,7 @@
         <v>10</v>
       </c>
       <c r="N3">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="O3">
         <v>30</v>
@@ -1990,10 +1992,10 @@
         <v>26</v>
       </c>
       <c r="Q3">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="R3">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="S3">
         <v>20</v>
@@ -2005,19 +2007,19 @@
         <v>10</v>
       </c>
       <c r="V3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="X3" s="7">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="Y3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -2026,7 +2028,7 @@
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>452</v>
+        <v>828</v>
       </c>
       <c r="E4" t="s">
         <v>26</v>
@@ -2056,7 +2058,7 @@
         <v>10</v>
       </c>
       <c r="N4">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="O4">
         <v>30</v>
@@ -2065,10 +2067,10 @@
         <v>26</v>
       </c>
       <c r="Q4">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="R4">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="S4">
         <v>20</v>
@@ -2080,19 +2082,19 @@
         <v>10</v>
       </c>
       <c r="V4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>140</v>
+        <v>160</v>
+      </c>
+      <c r="X4" s="7">
+        <v>160</v>
       </c>
       <c r="Y4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -2167,7 +2169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -2176,7 +2178,7 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -2215,7 +2217,7 @@
         <v>26</v>
       </c>
       <c r="Q6">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -2242,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -2251,7 +2253,7 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E7" t="s">
         <v>26</v>
@@ -2281,7 +2283,7 @@
         <v>1</v>
       </c>
       <c r="N7">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="O7">
         <v>6</v>
@@ -2290,10 +2292,10 @@
         <v>26</v>
       </c>
       <c r="Q7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S7">
         <v>3</v>
@@ -2311,13 +2313,13 @@
         <v>0</v>
       </c>
       <c r="X7" s="6">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="Y7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -2326,7 +2328,7 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="E8" t="s">
         <v>26</v>
@@ -2356,7 +2358,7 @@
         <v>1</v>
       </c>
       <c r="N8">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="O8">
         <v>20</v>
@@ -2368,7 +2370,7 @@
         <v>11</v>
       </c>
       <c r="R8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S8">
         <v>16</v>
@@ -2386,13 +2388,13 @@
         <v>0</v>
       </c>
       <c r="X8">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="Y8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -2467,7 +2469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -2542,7 +2544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -2617,7 +2619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2692,7 +2694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
@@ -2767,7 +2769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -2776,7 +2778,7 @@
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="E14" t="s">
         <v>26</v>
@@ -2806,7 +2808,7 @@
         <v>15</v>
       </c>
       <c r="N14">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="O14">
         <v>50</v>
@@ -2842,7 +2844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -2917,7 +2919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -2926,7 +2928,7 @@
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="E16" t="s">
         <v>26</v>
@@ -2956,7 +2958,7 @@
         <v>15</v>
       </c>
       <c r="N16">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="O16">
         <v>35</v>
@@ -2992,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -3067,7 +3069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -3076,7 +3078,7 @@
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="E18" t="s">
         <v>26</v>
@@ -3106,7 +3108,7 @@
         <v>15</v>
       </c>
       <c r="N18">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="O18">
         <v>35</v>
@@ -3142,7 +3144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -3217,7 +3219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -3292,7 +3294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -3367,7 +3369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -3442,7 +3444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -3451,7 +3453,7 @@
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E23" t="s">
         <v>26</v>
@@ -3508,7 +3510,7 @@
         <v>0</v>
       </c>
       <c r="W23">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="X23">
         <v>0</v>
@@ -3517,7 +3519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -3526,7 +3528,7 @@
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E24" t="s">
         <v>26</v>
@@ -3565,7 +3567,7 @@
         <v>26</v>
       </c>
       <c r="Q24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R24">
         <v>2</v>
@@ -3592,7 +3594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -3601,7 +3603,7 @@
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E25" t="s">
         <v>26</v>
@@ -3640,7 +3642,7 @@
         <v>26</v>
       </c>
       <c r="Q25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R25">
         <v>2</v>
@@ -3667,7 +3669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>69</v>
       </c>
@@ -3676,7 +3678,7 @@
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E26" t="s">
         <v>26</v>
@@ -3715,7 +3717,7 @@
         <v>26</v>
       </c>
       <c r="Q26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R26">
         <v>2</v>
@@ -3742,7 +3744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>71</v>
       </c>
@@ -3817,7 +3819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>72</v>
       </c>
@@ -3892,7 +3894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>74</v>
       </c>
@@ -3967,7 +3969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -3976,7 +3978,7 @@
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
-        <v>445</v>
+        <v>490</v>
       </c>
       <c r="E30" t="s">
         <v>26</v>
@@ -4006,7 +4008,7 @@
         <v>15</v>
       </c>
       <c r="N30">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="O30">
         <v>50</v>
@@ -4015,10 +4017,10 @@
         <v>26</v>
       </c>
       <c r="Q30">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="R30">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="S30">
         <v>0</v>
@@ -4042,7 +4044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -4051,7 +4053,7 @@
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
-        <v>445</v>
+        <v>490</v>
       </c>
       <c r="E31" t="s">
         <v>26</v>
@@ -4081,7 +4083,7 @@
         <v>15</v>
       </c>
       <c r="N31">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="O31">
         <v>50</v>
@@ -4090,10 +4092,10 @@
         <v>26</v>
       </c>
       <c r="Q31">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="R31">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="S31">
         <v>0</v>
@@ -4117,7 +4119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -4126,7 +4128,7 @@
       </c>
       <c r="D32">
         <f t="shared" si="0"/>
-        <v>445</v>
+        <v>490</v>
       </c>
       <c r="E32" t="s">
         <v>26</v>
@@ -4156,7 +4158,7 @@
         <v>15</v>
       </c>
       <c r="N32">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="O32">
         <v>50</v>
@@ -4165,10 +4167,10 @@
         <v>26</v>
       </c>
       <c r="Q32">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="R32">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="S32">
         <v>0</v>
@@ -4192,7 +4194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>81</v>
       </c>
@@ -4201,7 +4203,7 @@
       </c>
       <c r="D33">
         <f t="shared" si="0"/>
-        <v>445</v>
+        <v>490</v>
       </c>
       <c r="E33" t="s">
         <v>26</v>
@@ -4231,7 +4233,7 @@
         <v>15</v>
       </c>
       <c r="N33">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="O33">
         <v>50</v>
@@ -4240,10 +4242,10 @@
         <v>26</v>
       </c>
       <c r="Q33">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="R33">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="S33">
         <v>0</v>
@@ -4267,7 +4269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>83</v>
       </c>
@@ -4343,7 +4345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>85</v>
       </c>
@@ -4419,7 +4421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>86</v>
       </c>
@@ -4495,7 +4497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>88</v>
       </c>
@@ -4571,7 +4573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>90</v>
       </c>
@@ -4646,7 +4648,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>92</v>
       </c>
@@ -4721,7 +4723,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>94</v>
       </c>
@@ -4730,7 +4732,7 @@
       </c>
       <c r="D40">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E40" t="s">
         <v>26</v>
@@ -4760,7 +4762,7 @@
         <v>0</v>
       </c>
       <c r="N40">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O40">
         <v>3</v>
@@ -4793,10 +4795,10 @@
         <v>0</v>
       </c>
       <c r="Y40" s="6">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>95</v>
       </c>
@@ -4805,7 +4807,7 @@
       </c>
       <c r="D41">
         <f t="shared" si="1"/>
-        <v>207</v>
+        <v>248</v>
       </c>
       <c r="E41" t="s">
         <v>26</v>
@@ -4835,7 +4837,7 @@
         <v>0</v>
       </c>
       <c r="N41">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="O41">
         <v>30</v>
@@ -4859,7 +4861,7 @@
         <v>1</v>
       </c>
       <c r="V41">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="W41">
         <v>0</v>
@@ -4868,10 +4870,10 @@
         <v>0</v>
       </c>
       <c r="Y41" s="6">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>97</v>
       </c>
@@ -4946,7 +4948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>98</v>
       </c>
@@ -5021,7 +5023,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>99</v>
       </c>
@@ -5096,7 +5098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>101</v>
       </c>
@@ -5171,7 +5173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>103</v>
       </c>
@@ -5246,7 +5248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>105</v>
       </c>
@@ -5321,7 +5323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>107</v>
       </c>
@@ -5396,7 +5398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>109</v>
       </c>
@@ -5405,7 +5407,7 @@
       </c>
       <c r="D49">
         <f t="shared" si="1"/>
-        <v>228</v>
+        <v>258</v>
       </c>
       <c r="E49" t="s">
         <v>26</v>
@@ -5444,10 +5446,10 @@
         <v>26</v>
       </c>
       <c r="Q49">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="R49">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="S49">
         <v>1</v>
@@ -5471,7 +5473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>111</v>
       </c>
@@ -5480,7 +5482,7 @@
       </c>
       <c r="D50">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E50" t="s">
         <v>26</v>
@@ -5510,7 +5512,7 @@
         <v>0</v>
       </c>
       <c r="N50">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="O50">
         <v>0</v>
@@ -5546,7 +5548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>113</v>
       </c>
@@ -5621,7 +5623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>115</v>
       </c>
@@ -5696,7 +5698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>117</v>
       </c>
@@ -5771,7 +5773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>119</v>
       </c>
@@ -5846,7 +5848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>121</v>
       </c>
@@ -5921,7 +5923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>123</v>
       </c>
@@ -5996,7 +5998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>124</v>
       </c>
@@ -6071,7 +6073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>125</v>
       </c>
@@ -6146,7 +6148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>127</v>
       </c>
@@ -6221,7 +6223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>128</v>
       </c>
@@ -6296,7 +6298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>129</v>
       </c>
@@ -6371,7 +6373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>131</v>
       </c>
@@ -6446,7 +6448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>132</v>
       </c>
@@ -6521,7 +6523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>133</v>
       </c>
@@ -6596,7 +6598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>135</v>
       </c>
@@ -6671,7 +6673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>136</v>
       </c>
@@ -6746,7 +6748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>137</v>
       </c>
@@ -6821,7 +6823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>139</v>
       </c>
@@ -6896,7 +6898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>141</v>
       </c>
@@ -6971,7 +6973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>143</v>
       </c>
@@ -6980,7 +6982,7 @@
       </c>
       <c r="D70">
         <f t="shared" si="2"/>
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E70" t="s">
         <v>26</v>
@@ -7010,7 +7012,7 @@
         <v>0</v>
       </c>
       <c r="N70">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="O70">
         <v>30</v>
@@ -7046,7 +7048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>145</v>
       </c>
@@ -7121,7 +7123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>147</v>
       </c>
@@ -7196,7 +7198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>149</v>
       </c>
@@ -7271,7 +7273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>151</v>
       </c>
@@ -7346,7 +7348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>152</v>
       </c>
@@ -7421,7 +7423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>154</v>
       </c>
@@ -7496,7 +7498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>155</v>
       </c>
@@ -7571,7 +7573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>157</v>
       </c>
@@ -7580,38 +7582,38 @@
       </c>
       <c r="D78">
         <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="E78" t="s">
+        <v>26</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
+      <c r="L78">
+        <v>0</v>
+      </c>
+      <c r="M78">
+        <v>0</v>
+      </c>
+      <c r="N78">
         <v>45</v>
       </c>
-      <c r="E78" t="s">
-        <v>26</v>
-      </c>
-      <c r="F78">
-        <v>0</v>
-      </c>
-      <c r="G78">
-        <v>0</v>
-      </c>
-      <c r="H78">
-        <v>0</v>
-      </c>
-      <c r="I78">
-        <v>0</v>
-      </c>
-      <c r="J78">
-        <v>0</v>
-      </c>
-      <c r="K78">
-        <v>0</v>
-      </c>
-      <c r="L78">
-        <v>0</v>
-      </c>
-      <c r="M78">
-        <v>0</v>
-      </c>
-      <c r="N78">
-        <v>30</v>
-      </c>
       <c r="O78">
         <v>15</v>
       </c>
@@ -7646,7 +7648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>159</v>
       </c>
@@ -7655,7 +7657,7 @@
       </c>
       <c r="D79">
         <f t="shared" si="2"/>
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E79" t="s">
         <v>26</v>
@@ -7694,7 +7696,7 @@
         <v>26</v>
       </c>
       <c r="Q79">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="R79">
         <v>0</v>
@@ -7721,7 +7723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>161</v>
       </c>
@@ -7796,7 +7798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>163</v>
       </c>
@@ -7871,7 +7873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>165</v>
       </c>
@@ -7880,7 +7882,7 @@
       </c>
       <c r="D82">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E82" t="s">
         <v>26</v>
@@ -7919,7 +7921,7 @@
         <v>26</v>
       </c>
       <c r="Q82">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="R82">
         <v>0</v>
@@ -7946,7 +7948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>167</v>
       </c>
@@ -8021,7 +8023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>169</v>
       </c>
@@ -8096,7 +8098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>171</v>
       </c>
@@ -8171,7 +8173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>173</v>
       </c>
@@ -8246,7 +8248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>174</v>
       </c>
@@ -8321,7 +8323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>175</v>
       </c>
@@ -8396,7 +8398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>176</v>
       </c>
@@ -8471,7 +8473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>178</v>
       </c>
@@ -8546,7 +8548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>180</v>
       </c>
@@ -8621,7 +8623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>182</v>
       </c>
@@ -8696,7 +8698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>184</v>
       </c>
@@ -8771,7 +8773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>186</v>
       </c>
@@ -8847,7 +8849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>188</v>
       </c>
@@ -8922,7 +8924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>190</v>
       </c>
@@ -8931,7 +8933,7 @@
       </c>
       <c r="D96">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E96" t="s">
         <v>26</v>
@@ -8970,7 +8972,7 @@
         <v>26</v>
       </c>
       <c r="Q96">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R96">
         <v>2</v>
@@ -8997,7 +8999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>192</v>
       </c>
@@ -9006,7 +9008,7 @@
       </c>
       <c r="D97">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E97" t="s">
         <v>26</v>
@@ -9045,7 +9047,7 @@
         <v>26</v>
       </c>
       <c r="Q97">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R97">
         <v>2</v>
@@ -9072,7 +9074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>194</v>
       </c>
@@ -9081,7 +9083,7 @@
       </c>
       <c r="D98">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E98" t="s">
         <v>26</v>
@@ -9120,7 +9122,7 @@
         <v>26</v>
       </c>
       <c r="Q98">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R98">
         <v>2</v>
@@ -9147,7 +9149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>196</v>
       </c>
@@ -9222,7 +9224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>197</v>
       </c>
@@ -9297,7 +9299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>199</v>
       </c>
@@ -9372,7 +9374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>201</v>
       </c>
@@ -9447,7 +9449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>203</v>
       </c>
@@ -9522,7 +9524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>205</v>
       </c>
@@ -9597,7 +9599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>207</v>
       </c>
@@ -9672,7 +9674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>209</v>
       </c>
@@ -9681,7 +9683,7 @@
       </c>
       <c r="D106">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E106" t="s">
         <v>26</v>
@@ -9740,14 +9742,14 @@
       <c r="W106">
         <v>0</v>
       </c>
-      <c r="X106" s="6">
-        <v>4</v>
+      <c r="X106" s="8">
+        <v>3</v>
       </c>
       <c r="Y106" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>211</v>
       </c>
@@ -9822,7 +9824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>213</v>
       </c>
@@ -9897,7 +9899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>215</v>
       </c>
@@ -9972,7 +9974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>217</v>
       </c>
@@ -10047,7 +10049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>219</v>
       </c>
@@ -10122,7 +10124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>221</v>
       </c>
@@ -10197,7 +10199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>222</v>
       </c>
@@ -10272,7 +10274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>224</v>
       </c>
@@ -10347,7 +10349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>225</v>
       </c>
@@ -10422,7 +10424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>227</v>
       </c>
@@ -10431,7 +10433,7 @@
       </c>
       <c r="D116">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E116" t="s">
         <v>26</v>
@@ -10476,7 +10478,7 @@
         <v>0</v>
       </c>
       <c r="S116">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="T116">
         <v>0</v>
@@ -10497,7 +10499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>229</v>
       </c>
@@ -10572,7 +10574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>231</v>
       </c>
@@ -10647,7 +10649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>233</v>
       </c>
@@ -10722,7 +10724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>235</v>
       </c>
@@ -10797,7 +10799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>237</v>
       </c>
@@ -10872,7 +10874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>239</v>
       </c>
@@ -10947,7 +10949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>240</v>
       </c>
@@ -10956,7 +10958,7 @@
       </c>
       <c r="D123">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="E123" t="s">
         <v>26</v>
@@ -11001,16 +11003,16 @@
         <v>0</v>
       </c>
       <c r="S123">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T123">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U123">
-        <v>0</v>
-      </c>
-      <c r="V123">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="V123" s="8">
+        <v>11</v>
       </c>
       <c r="W123" s="6">
         <v>20</v>
@@ -11022,7 +11024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>241</v>
       </c>
@@ -11097,7 +11099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>243</v>
       </c>
@@ -11172,7 +11174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>245</v>
       </c>
@@ -11181,7 +11183,7 @@
       </c>
       <c r="D126">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E126" t="s">
         <v>26</v>
@@ -11220,7 +11222,7 @@
         <v>26</v>
       </c>
       <c r="Q126">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R126">
         <v>0</v>
@@ -11247,7 +11249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>247</v>
       </c>
@@ -11322,7 +11324,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>248</v>
       </c>
@@ -11397,7 +11399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>249</v>
       </c>
@@ -11472,7 +11474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>250</v>
       </c>
@@ -11547,7 +11549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>252</v>
       </c>
@@ -11622,7 +11624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>254</v>
       </c>
@@ -11698,10 +11700,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:Y132"/>
+  <autoFilter ref="C1:Y132" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C55" r:id="rId1"/>
+    <hyperlink ref="C55" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -11709,48 +11711,48 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AH60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="50.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="53.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="27" width="5.42578125" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="31" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="50.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="53.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.5546875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.88671875" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="7.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="6.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="5.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="27" width="5.44140625" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="31" width="11.33203125" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="33" max="33" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="19.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -11854,7 +11856,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>267</v>
       </c>
@@ -11959,7 +11961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>269</v>
       </c>
@@ -12064,7 +12066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>270</v>
       </c>
@@ -12169,7 +12171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>272</v>
       </c>
@@ -12274,7 +12276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>275</v>
       </c>
@@ -12379,7 +12381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>278</v>
       </c>
@@ -12484,7 +12486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>279</v>
       </c>
@@ -12589,7 +12591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>280</v>
       </c>
@@ -12598,7 +12600,7 @@
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>452</v>
+        <v>792</v>
       </c>
       <c r="E9" t="s">
         <v>26</v>
@@ -12682,16 +12684,16 @@
         <v>12</v>
       </c>
       <c r="AF9">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="AG9">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="AH9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>281</v>
       </c>
@@ -12793,7 +12795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>283</v>
       </c>
@@ -12895,7 +12897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>285</v>
       </c>
@@ -12997,7 +12999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>287</v>
       </c>
@@ -13099,7 +13101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>289</v>
       </c>
@@ -13201,7 +13203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>291</v>
       </c>
@@ -13303,7 +13305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>293</v>
       </c>
@@ -13405,7 +13407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>295</v>
       </c>
@@ -13507,7 +13509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>297</v>
       </c>
@@ -13609,7 +13611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>299</v>
       </c>
@@ -13711,7 +13713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>301</v>
       </c>
@@ -13813,7 +13815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>303</v>
       </c>
@@ -13915,7 +13917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>304</v>
       </c>
@@ -14017,7 +14019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>305</v>
       </c>
@@ -14119,7 +14121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>306</v>
       </c>
@@ -14221,7 +14223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>307</v>
       </c>
@@ -14323,7 +14325,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>308</v>
       </c>
@@ -14425,7 +14427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>309</v>
       </c>
@@ -14527,7 +14529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>310</v>
       </c>
@@ -14629,7 +14631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>311</v>
       </c>
@@ -14731,7 +14733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>312</v>
       </c>
@@ -14833,7 +14835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>313</v>
       </c>
@@ -14935,7 +14937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>314</v>
       </c>
@@ -15037,7 +15039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>315</v>
       </c>
@@ -15139,7 +15141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>317</v>
       </c>
@@ -15241,7 +15243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>319</v>
       </c>
@@ -15343,7 +15345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>321</v>
       </c>
@@ -15445,7 +15447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>323</v>
       </c>
@@ -15547,7 +15549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>325</v>
       </c>
@@ -15649,7 +15651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>327</v>
       </c>
@@ -15751,7 +15753,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>329</v>
       </c>
@@ -15853,7 +15855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>331</v>
       </c>
@@ -15955,7 +15957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>332</v>
       </c>
@@ -16057,7 +16059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>333</v>
       </c>
@@ -16159,7 +16161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>335</v>
       </c>
@@ -16261,7 +16263,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>337</v>
       </c>
@@ -16363,7 +16365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>338</v>
       </c>
@@ -16465,7 +16467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>340</v>
       </c>
@@ -16567,7 +16569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>342</v>
       </c>
@@ -16669,7 +16671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>344</v>
       </c>
@@ -16771,7 +16773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>346</v>
       </c>
@@ -16873,7 +16875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>347</v>
       </c>
@@ -16975,7 +16977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>348</v>
       </c>
@@ -17077,7 +17079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>349</v>
       </c>
@@ -17179,7 +17181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>351</v>
       </c>
@@ -17281,7 +17283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>352</v>
       </c>
@@ -17386,7 +17388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>355</v>
       </c>
@@ -17491,7 +17493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>358</v>
       </c>
@@ -17596,7 +17598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>361</v>
       </c>
@@ -17698,7 +17700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>417</v>
       </c>
@@ -17803,7 +17805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>418</v>
       </c>
@@ -17910,7 +17912,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B35" r:id="rId1" tooltip="Reliance Industries ~!@#$%^&amp;*()_+=-[]{}|;':,.&lt;&gt;/? Limited Reliance Industries" display="https://navatar61--tr2sb8.sandbox.lightning.force.com/lightning/r/0013C00000mphj3QAA/view"/>
+    <hyperlink ref="B35" r:id="rId1" tooltip="Reliance Industries ~!@#$%^&amp;*()_+=-[]{}|;':,.&lt;&gt;/? Limited Reliance Industries" display="https://navatar61--tr2sb8.sandbox.lightning.force.com/lightning/r/0013C00000mphj3QAA/view" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -17918,26 +17920,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="66.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="149.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="66.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="149.88671875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="119" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="149.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="149.88671875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="90" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="51.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="51.6640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -17963,7 +17965,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>370</v>
       </c>
@@ -17978,7 +17980,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>374</v>
       </c>
@@ -17987,7 +17989,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>376</v>
       </c>
@@ -18007,7 +18009,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>381</v>
       </c>
@@ -18016,7 +18018,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>383</v>
       </c>
@@ -18025,7 +18027,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>385</v>
       </c>
@@ -18036,7 +18038,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>387</v>
       </c>
@@ -18053,50 +18055,50 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AH5"/>
   <sheetViews>
     <sheetView topLeftCell="S1" workbookViewId="0">
       <selection activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21.6640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="7" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="26.85546875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="26.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="26.88671875" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="31" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="21.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="21.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="21.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="5.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="21.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="19.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="31" width="11.33203125" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="33" max="33" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="19.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -18200,7 +18202,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>388</v>
       </c>
@@ -18302,7 +18304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>389</v>
       </c>
@@ -18404,7 +18406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>390</v>
       </c>
@@ -18506,7 +18508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>391</v>
       </c>

</xml_diff>

<commit_message>
Updated test case file and acuity research data sheet
Signed-off-by: Nitin Garg <ngarg@navatargroup.com>
</commit_message>
<xml_diff>
--- a/ResearchDataSheet.xlsx
+++ b/ResearchDataSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nitin Garg\git\PE4.7Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A6F3E9-4B6D-4A90-A11E-9BB66981260C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BF5EF0-7F43-471E-BD46-8944B19DA65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4988" uniqueCount="1090">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4990" uniqueCount="1092">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -3314,6 +3314,12 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>AR_Up60</t>
+  </si>
+  <si>
+    <t>AR_Up61</t>
   </si>
 </sst>
 </file>
@@ -13712,8 +13718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AI63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20002,6 +20008,9 @@
       </c>
     </row>
     <row r="62" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>1090</v>
+      </c>
       <c r="B62">
         <v>56789012</v>
       </c>
@@ -20101,6 +20110,9 @@
       </c>
     </row>
     <row r="63" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>1091</v>
+      </c>
       <c r="B63">
         <v>56789012</v>
       </c>
@@ -20200,6 +20212,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B36" r:id="rId1" tooltip="Reliance Industries ~!@#$%^&amp;*()_+=-[]{}|;':,.&lt;&gt;/? Limited Reliance Industries" display="https://navatar61--tr2sb8.sandbox.lightning.force.com/lightning/r/0013C00000mphj3QAA/view" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Upadted acuity data sheet and research data sheet
Signed-off-by: Nitin Garg <ngarg@navatargroup.com>
</commit_message>
<xml_diff>
--- a/ResearchDataSheet.xlsx
+++ b/ResearchDataSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nitin Garg\git\PE4.7Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BF5EF0-7F43-471E-BD46-8944B19DA65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F226B83-3BBA-44DC-9713-E8CA5084E6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4990" uniqueCount="1092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4988" uniqueCount="1092">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -3767,7 +3767,7 @@
   <dimension ref="A1:Z132"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5457,7 +5457,7 @@
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
         <v>26</v>
@@ -5514,7 +5514,7 @@
         <v>0</v>
       </c>
       <c r="W23">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="X23">
         <v>0</v>
@@ -13718,8 +13718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AI63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:A63"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13859,9 +13859,7 @@
       <c r="AH1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AI1" s="2" t="s">
-        <v>1089</v>
-      </c>
+      <c r="AI1" s="2"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -17152,7 +17150,7 @@
       </c>
       <c r="D34">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E34" t="s">
         <v>26</v>
@@ -17224,7 +17222,7 @@
         <v>26</v>
       </c>
       <c r="AB34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC34">
         <v>1</v>
@@ -17239,7 +17237,7 @@
         <v>0</v>
       </c>
       <c r="AG34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH34">
         <v>0</v>
@@ -17356,7 +17354,7 @@
       </c>
       <c r="D36">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E36" t="s">
         <v>26</v>
@@ -17419,7 +17417,7 @@
         <v>26</v>
       </c>
       <c r="Y36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z36" t="s">
         <v>26</v>
@@ -17431,10 +17429,10 @@
         <v>1</v>
       </c>
       <c r="AC36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE36">
         <v>0</v>
@@ -17443,7 +17441,7 @@
         <v>0</v>
       </c>
       <c r="AG36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH36">
         <v>0</v>
@@ -17764,7 +17762,7 @@
       </c>
       <c r="D40">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E40" t="s">
         <v>26</v>
@@ -17854,7 +17852,7 @@
         <v>0</v>
       </c>
       <c r="AH40">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:34" x14ac:dyDescent="0.3">
@@ -20503,9 +20501,7 @@
       <c r="AH1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AI1" s="2" t="s">
-        <v>1089</v>
-      </c>
+      <c r="AI1" s="2"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" t="s">

</xml_diff>